<commit_message>
First static signpost in SignsTest added.
</commit_message>
<xml_diff>
--- a/Assets/Data Files/Choices.xlsx
+++ b/Assets/Data Files/Choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhoroszowski/workspace/HeartVan/Assets/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D64805-EAAF-2B4F-8171-E8C9E7CE0818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2695D00F-377D-A140-ACE8-030113555602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10500" yWindow="640" windowWidth="29980" windowHeight="13800" xr2:uid="{FC4FD709-265F-FD43-B075-E95662A0A2AF}"/>
   </bookViews>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2460BAA2-E8BE-1149-9077-8E747ECAEEE2}">
   <dimension ref="B1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,13 +1133,13 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Random sign data working
</commit_message>
<xml_diff>
--- a/Assets/Data Files/Choices.xlsx
+++ b/Assets/Data Files/Choices.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhoroszowski/workspace/HeartVan/Assets/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2695D00F-377D-A140-ACE8-030113555602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E4DFC9-2140-6E46-9891-148962957997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="640" windowWidth="29980" windowHeight="13800" xr2:uid="{FC4FD709-265F-FD43-B075-E95662A0A2AF}"/>
+    <workbookView xWindow="11840" yWindow="5680" windowWidth="32360" windowHeight="20600" xr2:uid="{FC4FD709-265F-FD43-B075-E95662A0A2AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="137">
   <si>
     <t>c_cat</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>f_overbite_sad</t>
+  </si>
+  <si>
+    <t>Line</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -496,13 +503,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8A633C1-3E24-7745-9CA6-ACB8248FB9CA}" name="Table1" displayName="Table1" ref="B1:E76" totalsRowShown="0">
-  <autoFilter ref="B1:E76" xr:uid="{090ACC27-16CF-FE48-B474-4BC7D16857CF}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8A633C1-3E24-7745-9CA6-ACB8248FB9CA}" name="Table1" displayName="Table1" ref="B1:F76" totalsRowShown="0">
+  <autoFilter ref="B1:F76" xr:uid="{090ACC27-16CF-FE48-B474-4BC7D16857CF}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{832CE5F6-90F8-7C43-B448-4D2F6117D128}" name="Choice"/>
     <tableColumn id="2" xr3:uid="{F577CB27-7045-F64A-BF13-2474BF825F10}" name="Option1"/>
     <tableColumn id="3" xr3:uid="{1D4F8CD0-96CB-5845-A1B5-CE8E044F0A51}" name="Option2"/>
     <tableColumn id="4" xr3:uid="{0CC0EAE2-38CF-5942-A1AE-5E7866AA5A83}" name="Option3"/>
+    <tableColumn id="5" xr3:uid="{13BCF18A-C785-DE4D-A158-15318CDE2D53}" name="Line" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -805,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2460BAA2-E8BE-1149-9077-8E747ECAEEE2}">
-  <dimension ref="B1:E76"/>
+  <dimension ref="B1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,10 +827,10 @@
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -833,8 +843,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -847,8 +860,12 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_cat", new Choice("f_devil", "f_heart_eyes", "f_shocked")},</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -861,8 +878,12 @@
       <c r="E3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_advocado", new Choice("f_sick_mask", "f_constipated_blush", "f_tongue_side")},</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -875,8 +896,12 @@
       <c r="E4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_america", new Choice("f_shades", "f_devil", "c_poop")},</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -889,8 +914,12 @@
       <c r="E5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_baby", new Choice("f_angel", "c_family", "f_sick_mask")},</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -903,8 +932,12 @@
       <c r="E6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_bacon", new Choice("f_crying", "f_smile", "f_disgusted")},</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -917,8 +950,12 @@
       <c r="E7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_banana", new Choice("c_eggplant", "f_tongue_out_close", "f_no_mouth")},</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -931,8 +968,12 @@
       <c r="E8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_bath", new Choice("c_surfing", "f_wink", "f_asleep")},</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -945,8 +986,12 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_bear", new Choice("f_side_eye_smile", "f_shocked_hands", "c_banana")},</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -959,8 +1004,12 @@
       <c r="E10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_beer", new Choice("f_heart_eyes", "c_police", "f_sad")},</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -973,8 +1022,12 @@
       <c r="E11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_bikini", new Choice("f_tongue_out_wink", "f_o_face", "f_disgusted")},</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -987,8 +1040,12 @@
       <c r="E12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_birthday_cake", new Choice("f_upside_down", "f_shocked", "f_kiss")},</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -1001,8 +1058,12 @@
       <c r="E13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_building_broken", new Choice("c_america", "f_crying", "f_worried")},</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -1015,8 +1076,12 @@
       <c r="E14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_burger", new Choice("f_blank", "f_content", "c_horse")},</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1029,8 +1094,12 @@
       <c r="E15" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_cancer", new Choice("c_island", "f_overbite", "f_smoke_nose")},</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -1043,8 +1112,12 @@
       <c r="E16" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_cheese", new Choice("f_sparkle_eye_cry", "f_smile", "f_grimace")},</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1057,8 +1130,12 @@
       <c r="E17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_christmas_tree", new Choice("f_frown_simple", "f_blush", "f_smile+intense")},</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1071,8 +1148,12 @@
       <c r="E18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_coffin", new Choice("c_cancer", "c_smoking", "c_rocket")},</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -1085,8 +1166,12 @@
       <c r="E19" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_cookie", new Choice("c_radiation", "f_overbite_shocked", "f_smile_simple")},</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -1099,8 +1184,12 @@
       <c r="E20" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_crown", new Choice("f_angry_red", "f_side_eyes_frown", "f_tongue_out")},</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -1113,8 +1202,12 @@
       <c r="E21" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_cupid_heart", new Choice("f_angel", "f_shout", "f_shock_sweat")},</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -1127,8 +1220,12 @@
       <c r="E22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_desert", new Choice("f_nose_bubble", "f_devil", "c_ice_cream")},</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>29</v>
       </c>
@@ -1141,8 +1238,12 @@
       <c r="E23" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_donut", new Choice("f_heart_eyes", "c_police", "f_overbite_shocked")},</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>30</v>
       </c>
@@ -1155,8 +1256,12 @@
       <c r="E24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_eggplant", new Choice("f_heart_eyes", "c_horse", "f_shocked")},</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>31</v>
       </c>
@@ -1169,8 +1274,12 @@
       <c r="E25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_family", new Choice("f_sick_mask", "c_prayer", "f_heart_eyes")},</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -1183,8 +1292,12 @@
       <c r="E26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_gay_kiss", new Choice("c_prayer", "f_kiss_heart", "c_ice_cream")},</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>33</v>
       </c>
@@ -1197,8 +1310,12 @@
       <c r="E27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_goat", new Choice("f_grimace", "f_content", "c_bacon")},</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -1211,8 +1328,12 @@
       <c r="E28" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_green_tea", new Choice("f_smile_simple", "f_disgusted", "f_blank")},</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -1225,8 +1346,12 @@
       <c r="E29" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_high_heel", new Choice("c_lesbian_kiss", "f_o_face", "f_content")},</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>36</v>
       </c>
@@ -1239,8 +1364,12 @@
       <c r="E30" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_horse", new Choice("f_worried", "f_crying", "f_wink")},</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>37</v>
       </c>
@@ -1253,8 +1382,12 @@
       <c r="E31" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_hospital", new Choice("f_sick_mask", "f_worried_sweat", "f_angel")},</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>38</v>
       </c>
@@ -1267,8 +1400,12 @@
       <c r="E32" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_ice_cream", new Choice("f_tongue_side", "c_rainbow", "f_angry")},</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -1281,8 +1418,12 @@
       <c r="E33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_island", new Choice("f_blank_closed_eyes", "f_kiss_heart", "f_smile_sweat")},</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>40</v>
       </c>
@@ -1295,8 +1436,12 @@
       <c r="E34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_jack_o_lantern", new Choice("c_police", "f_blank_eyes", "f_shout")},</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>41</v>
       </c>
@@ -1309,8 +1454,12 @@
       <c r="E35" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_king", new Choice("c_queen", "f_kiss", "c_leo")},</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>42</v>
       </c>
@@ -1323,8 +1472,12 @@
       <c r="E36" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_leo", new Choice("f_dead_eyes", "c_wolf", "f_smile_sweat")},</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>43</v>
       </c>
@@ -1337,8 +1490,12 @@
       <c r="E37" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_lesbian_kiss", new Choice("c_lips", "f_wide_smile", "c_rocket")},</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>44</v>
       </c>
@@ -1351,8 +1508,12 @@
       <c r="E38" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_lips", new Choice("f_kiss_heart", "f_upside_down", "c_taco")},</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>45</v>
       </c>
@@ -1365,8 +1526,12 @@
       <c r="E39" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_middle_finger", new Choice("f_shocked_hands", "c_police", "f_content")},</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>46</v>
       </c>
@@ -1379,8 +1544,12 @@
       <c r="E40" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_monkey", new Choice("f_asleep", "f_smile_teeth", "f_worried")},</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>47</v>
       </c>
@@ -1393,8 +1562,12 @@
       <c r="E41" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_no_smoking", new Choice("f_shades", "f_angry_red", "f_blank")},</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>48</v>
       </c>
@@ -1407,8 +1580,12 @@
       <c r="E42" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_pancakes", new Choice("f_smile_wide", "f_no_mouth", "f_frown_simple")},</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>49</v>
       </c>
@@ -1421,8 +1598,12 @@
       <c r="E43" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_peace", new Choice("c_surfing", "c_king", "c_rocket")},</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>50</v>
       </c>
@@ -1435,8 +1616,12 @@
       <c r="E44" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_peace_sign", new Choice("c_middle_finger", "f_smoke_nose", "f_o_face_eyebrows")},</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>51</v>
       </c>
@@ -1449,8 +1634,12 @@
       <c r="E45" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_piggie", new Choice("c_bacon", "f_kiss_eyes", "c_police")},</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>52</v>
       </c>
@@ -1463,8 +1652,12 @@
       <c r="E46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_pizza", new Choice("f_worried", "f_heart_eyes", "c_beer")},</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>53</v>
       </c>
@@ -1477,8 +1670,12 @@
       <c r="E47" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_police", new Choice("c_queen", "c_piggie", "c_king")},</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>54</v>
       </c>
@@ -1491,8 +1688,12 @@
       <c r="E48" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_poop", new Choice("c_ice_cream", "f_disgusted", "c_taco")},</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>55</v>
       </c>
@@ -1505,8 +1706,12 @@
       <c r="E49" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_prayer", new Choice("f_devil", "f_upside_down", "f_angel")},</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>56</v>
       </c>
@@ -1519,8 +1724,12 @@
       <c r="E50" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_present", new Choice("f_blush", "c_birthday_cake", "f_tongue_out")},</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>57</v>
       </c>
@@ -1533,8 +1742,12 @@
       <c r="E51" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_queen", new Choice("f_heart_eyes", "f_shades", "c_bath")},</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>58</v>
       </c>
@@ -1547,8 +1760,12 @@
       <c r="E52" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_rabbit", new Choice("c_wolf", "f_content", "f_blank_eyes")},</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>59</v>
       </c>
@@ -1561,8 +1778,12 @@
       <c r="E53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_radiation", new Choice("f_shocked_hands", "c_peace", "f_sick_mask")},</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>60</v>
       </c>
@@ -1575,8 +1796,12 @@
       <c r="E54" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_rainbow", new Choice("c_police", "c_gay_kiss", "c_high_heel")},</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>61</v>
       </c>
@@ -1589,8 +1814,12 @@
       <c r="E55" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_recycle", new Choice("c_volcano", "c_sun_ocean", "f_smile_simple")},</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>62</v>
       </c>
@@ -1603,8 +1832,12 @@
       <c r="E56" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_rocket", new Choice("f_dead_eyes", "f_shades", "c_banana")},</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>63</v>
       </c>
@@ -1617,8 +1850,12 @@
       <c r="E57" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_rooster", new Choice("c_burger", "f_shocked_blush", "c_rocket")},</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>64</v>
       </c>
@@ -1631,8 +1868,12 @@
       <c r="E58" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_rowing", new Choice("f_asleep", "f_smoke_nose", "c_taxi")},</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>65</v>
       </c>
@@ -1645,8 +1886,12 @@
       <c r="E59" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_saki", new Choice("c_wine", "f_blush", "c_green_tea")},</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>66</v>
       </c>
@@ -1659,8 +1904,12 @@
       <c r="E60" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_salad", new Choice("f_tounge_side", "c_rabbit", "c_burger")},</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>67</v>
       </c>
@@ -1673,8 +1922,12 @@
       <c r="E61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_shrimp", new Choice("c_sun_ocean", "f_disgusted", "f_heart_eyes")},</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>68</v>
       </c>
@@ -1687,8 +1940,12 @@
       <c r="E62" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F62" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_smoking", new Choice("f_no_mouth", "f_smile", "f_dead_eyes")},</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>69</v>
       </c>
@@ -1701,8 +1958,12 @@
       <c r="E63" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F63" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_sun_mountain", new Choice("c_goat", "c_king", "f_smoke_nose")},</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>70</v>
       </c>
@@ -1715,8 +1976,12 @@
       <c r="E64" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F64" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_sun_ocean", new Choice("f_smile_eyes", "c_island", "c_shrimp")},</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>71</v>
       </c>
@@ -1729,8 +1994,12 @@
       <c r="E65" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F65" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_surfing", new Choice("f_asleep", "f_wink", "c_bikini")},</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>72</v>
       </c>
@@ -1743,8 +2012,12 @@
       <c r="E66" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F66" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_sushi", new Choice("c_green_tea", "f_shades", "f_disgusted")},</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>73</v>
       </c>
@@ -1757,8 +2030,12 @@
       <c r="E67" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F67" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_swords", new Choice("c_hospital", "f_angry_red", "f_shock_sweat")},</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>74</v>
       </c>
@@ -1771,8 +2048,12 @@
       <c r="E68" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F68" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_taco", new Choice("c_poop", "f_kiss_blush", "c_burger")},</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>75</v>
       </c>
@@ -1785,8 +2066,12 @@
       <c r="E69" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F69" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_taxi", new Choice("f_asleep", "f_worried", "c_rowing")},</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>76</v>
       </c>
@@ -1799,8 +2084,12 @@
       <c r="E70" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F70" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_tiger", new Choice("c_cat", "f_shades", "c_leo")},</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>77</v>
       </c>
@@ -1813,8 +2102,12 @@
       <c r="E71" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F71" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_tongue", new Choice("c_burger", "c_pancakes", "c_pizza")},</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>78</v>
       </c>
@@ -1827,8 +2120,12 @@
       <c r="E72" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F72" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_trophy", new Choice("c_horse", "f_overbite_sad", "f_smile_teeth")},</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>79</v>
       </c>
@@ -1841,8 +2138,12 @@
       <c r="E73" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F73" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_volcano", new Choice("f_shocked", "c_recycle", "c_smoking")},</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>80</v>
       </c>
@@ -1855,8 +2156,12 @@
       <c r="E74" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F74" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_wine", new Choice("c_lips", "c_bath", "f_no_mouth")},</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>81</v>
       </c>
@@ -1869,8 +2174,12 @@
       <c r="E75" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F75" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_wolf", new Choice("c_rabbit", "f_heart_eyes", "f_overbite")},</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>82</v>
       </c>
@@ -1882,6 +2191,10 @@
       </c>
       <c r="E76" t="s">
         <v>1</v>
+      </c>
+      <c r="F76" t="str">
+        <f>_xlfn.CONCAT("{""",Table1[[#This Row],[Choice]],""", new Choice(""",Table1[[#This Row],[Option1]],""", """,Table1[[#This Row],[Option2]],""", """,Table1[[#This Row],[Option3]],""")},")</f>
+        <v>{"c_ying_yang", new Choice("f_angel", "c_cat", "f_devil")},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>